<commit_message>
add some label data
</commit_message>
<xml_diff>
--- a/SentimentLineFig/accuracy.xlsx
+++ b/SentimentLineFig/accuracy.xlsx
@@ -112,7 +112,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -126,6 +126,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F10"/>
+  <dimension ref="B3:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:F10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -439,7 +442,7 @@
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>1154</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -450,7 +453,7 @@
       </c>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D5" s="5"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
@@ -470,24 +473,27 @@
       </c>
     </row>
     <row r="9" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>87642</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="3">
-        <v>18.191449251000002</v>
+      <c r="F9" s="5">
+        <v>146.88193332</v>
       </c>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D10" s="5"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="3">
-        <v>146.88193332</v>
-      </c>
+      <c r="F10" s="5">
+        <v>18.191449251000002</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>